<commit_message>
Updated search to be more general
</commit_message>
<xml_diff>
--- a/resources/Finnhub Exchanges.xlsx
+++ b/resources/Finnhub Exchanges.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C549F6-DEB5-4424-802C-4D4DE6577DBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Trang tính1" sheetId="1" r:id="rId4"/>
+    <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="359">
   <si>
     <t>code</t>
   </si>
@@ -1085,43 +1094,54 @@
   </si>
   <si>
     <t>https://www.tradinghours.com/exchanges/gpw</t>
+  </si>
+  <si>
+    <t>priority</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF1155CC"/>
-    </font>
-    <font>
-      <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1129,54 +1149,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1366,24 +1383,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="70.0"/>
-    <col customWidth="1" min="4" max="4" width="28.43"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1408,8 +1432,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="I1" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1430,7 +1457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1451,7 +1478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1473,8 +1500,11 @@
       <c r="H4" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1495,7 +1525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1516,7 +1546,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1537,7 +1567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1558,7 +1588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1579,7 +1609,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1602,7 +1632,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
@@ -1623,7 +1653,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1643,8 +1673,11 @@
       <c r="H12" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="I12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1664,8 +1697,11 @@
       <c r="H13" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="I13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>82</v>
       </c>
@@ -1686,7 +1722,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -1706,8 +1742,11 @@
       <c r="H15" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="I15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
@@ -1730,7 +1769,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
@@ -1751,7 +1790,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -1773,8 +1812,11 @@
       <c r="H18" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="I18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>107</v>
       </c>
@@ -1794,8 +1836,11 @@
       <c r="H19" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="I19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>113</v>
       </c>
@@ -1815,8 +1860,11 @@
       <c r="H20" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="I20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>119</v>
       </c>
@@ -1837,7 +1885,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
@@ -1857,8 +1905,11 @@
       <c r="H22" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="I22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>129</v>
       </c>
@@ -1879,7 +1930,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>134</v>
       </c>
@@ -1900,7 +1951,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>140</v>
       </c>
@@ -1921,7 +1972,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>146</v>
       </c>
@@ -1942,7 +1993,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>151</v>
       </c>
@@ -1963,7 +2014,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -1985,8 +2036,11 @@
       <c r="H28" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="I28">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>164</v>
       </c>
@@ -2008,8 +2062,11 @@
       <c r="H29" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="I29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>169</v>
       </c>
@@ -2031,8 +2088,11 @@
       <c r="H30" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="31">
+      <c r="I30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2053,7 +2113,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>181</v>
       </c>
@@ -2074,7 +2134,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>186</v>
       </c>
@@ -2095,7 +2155,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>192</v>
       </c>
@@ -2116,7 +2176,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>198</v>
       </c>
@@ -2137,7 +2197,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>202</v>
       </c>
@@ -2158,7 +2218,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>208</v>
       </c>
@@ -2179,7 +2239,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>214</v>
       </c>
@@ -2202,7 +2262,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>218</v>
       </c>
@@ -2222,8 +2282,11 @@
       <c r="H39" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="40">
+      <c r="I39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>224</v>
       </c>
@@ -2244,7 +2307,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>230</v>
       </c>
@@ -2265,7 +2328,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>235</v>
       </c>
@@ -2285,8 +2348,11 @@
       <c r="H42" s="4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="43">
+      <c r="I42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>240</v>
       </c>
@@ -2307,7 +2373,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>246</v>
       </c>
@@ -2328,7 +2394,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>252</v>
       </c>
@@ -2349,7 +2415,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>258</v>
       </c>
@@ -2370,7 +2436,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>263</v>
       </c>
@@ -2391,7 +2457,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>269</v>
       </c>
@@ -2412,7 +2478,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>274</v>
       </c>
@@ -2438,7 +2504,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>280</v>
       </c>
@@ -2459,7 +2525,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>286</v>
       </c>
@@ -2479,8 +2545,11 @@
       <c r="H51" s="4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="52">
+      <c r="I51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>291</v>
       </c>
@@ -2500,8 +2569,11 @@
       <c r="H52" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="53">
+      <c r="I52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>296</v>
       </c>
@@ -2521,8 +2593,11 @@
       <c r="H53" s="4" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="54">
+      <c r="I53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>302</v>
       </c>
@@ -2542,8 +2617,11 @@
       <c r="H54" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="55">
+      <c r="I54">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>308</v>
       </c>
@@ -2567,7 +2645,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>314</v>
       </c>
@@ -2588,7 +2666,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>319</v>
       </c>
@@ -2608,8 +2686,11 @@
       <c r="H57" s="4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="58">
+      <c r="I57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>323</v>
       </c>
@@ -2632,7 +2713,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>328</v>
       </c>
@@ -2653,8 +2734,11 @@
       <c r="H59" s="4" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="60">
+      <c r="I59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>332</v>
       </c>
@@ -2675,7 +2759,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>337</v>
       </c>
@@ -2695,8 +2779,11 @@
       <c r="H61" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="62">
+      <c r="I61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>343</v>
       </c>
@@ -2717,7 +2804,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>347</v>
       </c>
@@ -2738,7 +2825,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>352</v>
       </c>
@@ -2758,83 +2845,86 @@
       <c r="H64" s="4" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="65">
+      <c r="I64">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="H2"/>
-    <hyperlink r:id="rId2" ref="H3"/>
-    <hyperlink r:id="rId3" ref="H4"/>
-    <hyperlink r:id="rId4" ref="H5"/>
-    <hyperlink r:id="rId5" ref="H6"/>
-    <hyperlink r:id="rId6" ref="H7"/>
-    <hyperlink r:id="rId7" ref="H8"/>
-    <hyperlink r:id="rId8" ref="H9"/>
-    <hyperlink r:id="rId9" ref="H10"/>
-    <hyperlink r:id="rId10" ref="H11"/>
-    <hyperlink r:id="rId11" ref="H12"/>
-    <hyperlink r:id="rId12" ref="H13"/>
-    <hyperlink r:id="rId13" ref="H14"/>
-    <hyperlink r:id="rId14" ref="H15"/>
-    <hyperlink r:id="rId15" ref="H16"/>
-    <hyperlink r:id="rId16" ref="H17"/>
-    <hyperlink r:id="rId17" ref="H18"/>
-    <hyperlink r:id="rId18" ref="H19"/>
-    <hyperlink r:id="rId19" ref="H20"/>
-    <hyperlink r:id="rId20" ref="H21"/>
-    <hyperlink r:id="rId21" ref="H22"/>
-    <hyperlink r:id="rId22" ref="H23"/>
-    <hyperlink r:id="rId23" ref="H24"/>
-    <hyperlink r:id="rId24" ref="H25"/>
-    <hyperlink r:id="rId25" ref="H26"/>
-    <hyperlink r:id="rId26" ref="H27"/>
-    <hyperlink r:id="rId27" ref="H28"/>
-    <hyperlink r:id="rId28" ref="H29"/>
-    <hyperlink r:id="rId29" ref="H30"/>
-    <hyperlink r:id="rId30" ref="H31"/>
-    <hyperlink r:id="rId31" ref="H32"/>
-    <hyperlink r:id="rId32" ref="H33"/>
-    <hyperlink r:id="rId33" ref="H34"/>
-    <hyperlink r:id="rId34" ref="H35"/>
-    <hyperlink r:id="rId35" ref="H36"/>
-    <hyperlink r:id="rId36" ref="H37"/>
-    <hyperlink r:id="rId37" ref="H38"/>
-    <hyperlink r:id="rId38" ref="H39"/>
-    <hyperlink r:id="rId39" ref="H40"/>
-    <hyperlink r:id="rId40" ref="H41"/>
-    <hyperlink r:id="rId41" ref="H42"/>
-    <hyperlink r:id="rId42" ref="H43"/>
-    <hyperlink r:id="rId43" ref="H44"/>
-    <hyperlink r:id="rId44" ref="H45"/>
-    <hyperlink r:id="rId45" ref="H46"/>
-    <hyperlink r:id="rId46" ref="H47"/>
-    <hyperlink r:id="rId47" ref="H48"/>
-    <hyperlink r:id="rId48" ref="H49"/>
-    <hyperlink r:id="rId49" ref="D50"/>
-    <hyperlink r:id="rId50" ref="H50"/>
-    <hyperlink r:id="rId51" ref="H51"/>
-    <hyperlink r:id="rId52" ref="H52"/>
-    <hyperlink r:id="rId53" ref="H53"/>
-    <hyperlink r:id="rId54" ref="H54"/>
-    <hyperlink r:id="rId55" ref="H55"/>
-    <hyperlink r:id="rId56" ref="H56"/>
-    <hyperlink r:id="rId57" ref="H57"/>
-    <hyperlink r:id="rId58" ref="H58"/>
-    <hyperlink r:id="rId59" ref="H59"/>
-    <hyperlink r:id="rId60" ref="H60"/>
-    <hyperlink r:id="rId61" ref="H61"/>
-    <hyperlink r:id="rId62" ref="D62"/>
-    <hyperlink r:id="rId63" ref="H62"/>
-    <hyperlink r:id="rId64" ref="H63"/>
-    <hyperlink r:id="rId65" ref="H64"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="H26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="H40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="H45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="H47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="H48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="H49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="H50" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="H51" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="H52" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="H53" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="H54" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="H55" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="H56" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="H57" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="H58" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="H59" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H60" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="H61" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D62" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="H62" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="H63" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="H64" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
   </hyperlinks>
-  <drawing r:id="rId66"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed database watchlist relationship. Watchlist api running. Broke the database for portfolio
</commit_message>
<xml_diff>
--- a/resources/Finnhub Exchanges.xlsx
+++ b/resources/Finnhub Exchanges.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644A1FE7-BAD3-4554-B258-46CB188EFE99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385D69C8-A70A-4A2A-87BD-1EB0F89498B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Trang tính1'!$A$1:$H$64</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1390,21 +1393,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="51.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1436,7 +1439,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1499,9 +1502,6 @@
       </c>
       <c r="H4" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1546,7 +1546,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
@@ -1674,10 +1674,10 @@
         <v>75</v>
       </c>
       <c r="I12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1697,9 +1697,6 @@
       <c r="H13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I13">
-        <v>21</v>
-      </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1722,7 +1719,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -1742,11 +1739,8 @@
       <c r="H15" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
@@ -1769,7 +1763,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
@@ -1790,7 +1784,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -1812,11 +1806,8 @@
       <c r="H18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>107</v>
       </c>
@@ -1836,11 +1827,8 @@
       <c r="H19" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>113</v>
       </c>
@@ -1860,11 +1848,8 @@
       <c r="H20" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>119</v>
       </c>
@@ -1885,7 +1870,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
@@ -1905,11 +1890,8 @@
       <c r="H22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I22">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>129</v>
       </c>
@@ -1930,7 +1912,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>134</v>
       </c>
@@ -1951,7 +1933,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>140</v>
       </c>
@@ -1972,7 +1954,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>146</v>
       </c>
@@ -1993,7 +1975,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>151</v>
       </c>
@@ -2014,7 +1996,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -2036,11 +2018,8 @@
       <c r="H28" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="I28">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>164</v>
       </c>
@@ -2062,11 +2041,8 @@
       <c r="H29" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I29">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>169</v>
       </c>
@@ -2088,11 +2064,8 @@
       <c r="H30" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="I30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2113,7 +2086,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>181</v>
       </c>
@@ -2134,7 +2107,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>186</v>
       </c>
@@ -2155,7 +2128,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>192</v>
       </c>
@@ -2176,7 +2149,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>198</v>
       </c>
@@ -2197,7 +2170,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>202</v>
       </c>
@@ -2218,7 +2191,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>208</v>
       </c>
@@ -2239,7 +2212,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>214</v>
       </c>
@@ -2262,7 +2235,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>218</v>
       </c>
@@ -2282,11 +2255,8 @@
       <c r="H39" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="I39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>224</v>
       </c>
@@ -2307,7 +2277,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>230</v>
       </c>
@@ -2328,7 +2298,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>235</v>
       </c>
@@ -2348,11 +2318,8 @@
       <c r="H42" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="I42">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>240</v>
       </c>
@@ -2373,7 +2340,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>246</v>
       </c>
@@ -2394,7 +2361,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>252</v>
       </c>
@@ -2415,7 +2382,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>258</v>
       </c>
@@ -2436,7 +2403,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>263</v>
       </c>
@@ -2457,7 +2424,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>269</v>
       </c>
@@ -2478,7 +2445,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>274</v>
       </c>
@@ -2504,7 +2471,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>280</v>
       </c>
@@ -2525,7 +2492,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>286</v>
       </c>
@@ -2545,11 +2512,8 @@
       <c r="H51" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="I51">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>291</v>
       </c>
@@ -2569,11 +2533,8 @@
       <c r="H52" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I52">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>296</v>
       </c>
@@ -2593,11 +2554,8 @@
       <c r="H53" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="I53">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>302</v>
       </c>
@@ -2617,11 +2575,8 @@
       <c r="H54" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="I54">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>308</v>
       </c>
@@ -2645,7 +2600,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>314</v>
       </c>
@@ -2686,11 +2641,8 @@
       <c r="H57" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="I57">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>323</v>
       </c>
@@ -2735,7 +2687,7 @@
         <v>331</v>
       </c>
       <c r="I59">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2759,7 +2711,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>337</v>
       </c>
@@ -2779,11 +2731,8 @@
       <c r="H61" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="I61">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>343</v>
       </c>
@@ -2804,7 +2753,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>347</v>
       </c>
@@ -2825,7 +2774,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>352</v>
       </c>
@@ -2845,9 +2794,6 @@
       <c r="H64" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="I64">
-        <v>13</v>
-      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
@@ -2858,6 +2804,20 @@
       <c r="B66" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H64" xr:uid="{40A68074-9A5C-43EE-8DF8-07B17DFBE83F}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="America/Argentina/Buenos_Aires"/>
+        <filter val="America/Caracas"/>
+        <filter val="America/Cuiaba"/>
+        <filter val="America/Mexico_City"/>
+        <filter val="America/New_York"/>
+        <filter val="America/Santiago"/>
+        <filter val="America/Sao_Paulo"/>
+        <filter val="America/Toronto"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
Updated database and market order endpoint. Fixed broken endpoints from earlier changes. Finished database relationships (for now)
</commit_message>
<xml_diff>
--- a/resources/Finnhub Exchanges.xlsx
+++ b/resources/Finnhub Exchanges.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385D69C8-A70A-4A2A-87BD-1EB0F89498B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644A1FE7-BAD3-4554-B258-46CB188EFE99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Trang tính1'!$A$1:$H$64</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1393,21 +1390,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="51.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1439,7 +1436,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1502,6 +1499,9 @@
       </c>
       <c r="H4" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1546,7 +1546,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
@@ -1674,10 +1674,10 @@
         <v>75</v>
       </c>
       <c r="I12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1697,6 +1697,9 @@
       <c r="H13" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="I13">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1719,7 +1722,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
@@ -1739,8 +1742,11 @@
       <c r="H15" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
@@ -1763,7 +1769,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
@@ -1784,7 +1790,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -1806,8 +1812,11 @@
       <c r="H18" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>107</v>
       </c>
@@ -1827,8 +1836,11 @@
       <c r="H19" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>113</v>
       </c>
@@ -1848,8 +1860,11 @@
       <c r="H20" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>119</v>
       </c>
@@ -1870,7 +1885,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
@@ -1890,8 +1905,11 @@
       <c r="H22" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>129</v>
       </c>
@@ -1912,7 +1930,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>134</v>
       </c>
@@ -1933,7 +1951,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>140</v>
       </c>
@@ -1954,7 +1972,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>146</v>
       </c>
@@ -1975,7 +1993,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>151</v>
       </c>
@@ -1996,7 +2014,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -2018,8 +2036,11 @@
       <c r="H28" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>164</v>
       </c>
@@ -2041,8 +2062,11 @@
       <c r="H29" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>169</v>
       </c>
@@ -2064,8 +2088,11 @@
       <c r="H30" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2086,7 +2113,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>181</v>
       </c>
@@ -2107,7 +2134,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>186</v>
       </c>
@@ -2128,7 +2155,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>192</v>
       </c>
@@ -2149,7 +2176,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>198</v>
       </c>
@@ -2170,7 +2197,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>202</v>
       </c>
@@ -2191,7 +2218,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>208</v>
       </c>
@@ -2212,7 +2239,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>214</v>
       </c>
@@ -2235,7 +2262,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>218</v>
       </c>
@@ -2255,8 +2282,11 @@
       <c r="H39" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>224</v>
       </c>
@@ -2277,7 +2307,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>230</v>
       </c>
@@ -2298,7 +2328,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>235</v>
       </c>
@@ -2318,8 +2348,11 @@
       <c r="H42" s="4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>240</v>
       </c>
@@ -2340,7 +2373,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>246</v>
       </c>
@@ -2361,7 +2394,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>252</v>
       </c>
@@ -2382,7 +2415,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>258</v>
       </c>
@@ -2403,7 +2436,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>263</v>
       </c>
@@ -2424,7 +2457,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>269</v>
       </c>
@@ -2445,7 +2478,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>274</v>
       </c>
@@ -2471,7 +2504,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>280</v>
       </c>
@@ -2492,7 +2525,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>286</v>
       </c>
@@ -2512,8 +2545,11 @@
       <c r="H51" s="4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>291</v>
       </c>
@@ -2533,8 +2569,11 @@
       <c r="H52" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>296</v>
       </c>
@@ -2554,8 +2593,11 @@
       <c r="H53" s="4" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>302</v>
       </c>
@@ -2575,8 +2617,11 @@
       <c r="H54" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>308</v>
       </c>
@@ -2600,7 +2645,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>314</v>
       </c>
@@ -2641,8 +2686,11 @@
       <c r="H57" s="4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>323</v>
       </c>
@@ -2687,7 +2735,7 @@
         <v>331</v>
       </c>
       <c r="I59">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2711,7 +2759,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>337</v>
       </c>
@@ -2731,8 +2779,11 @@
       <c r="H61" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>343</v>
       </c>
@@ -2753,7 +2804,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>347</v>
       </c>
@@ -2774,7 +2825,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>352</v>
       </c>
@@ -2794,6 +2845,9 @@
       <c r="H64" s="4" t="s">
         <v>357</v>
       </c>
+      <c r="I64">
+        <v>13</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
@@ -2804,20 +2858,6 @@
       <c r="B66" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H64" xr:uid="{40A68074-9A5C-43EE-8DF8-07B17DFBE83F}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="America/Argentina/Buenos_Aires"/>
-        <filter val="America/Caracas"/>
-        <filter val="America/Cuiaba"/>
-        <filter val="America/Mexico_City"/>
-        <filter val="America/New_York"/>
-        <filter val="America/Santiago"/>
-        <filter val="America/Sao_Paulo"/>
-        <filter val="America/Toronto"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>